<commit_message>
Expanded Preprocess for Induction Loop data
</commit_message>
<xml_diff>
--- a/03_Mapping/Vehicle_Type_Mapping.xlsx
+++ b/03_Mapping/Vehicle_Type_Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailunimannheimde-my.sharepoint.com/personal/pstapf_mail_uni-mannheim_de/Documents/Uni/Master/Semester 3/Teamproject/Towards-Sustainable-Cities-through-Simulation/03_Mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="158" documentId="11_AD4DB114E441178AC67DF4B50ED1E6EA693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCBB1EC9-9241-4A5D-A294-81815A0FD601}"/>
+  <xr:revisionPtr revIDLastSave="164" documentId="11_AD4DB114E441178AC67DF4B50ED1E6EA693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53A88ABC-D9C6-4674-865A-E1605C90D3E7}"/>
   <bookViews>
-    <workbookView xWindow="1665" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
   <si>
     <t>PKW (S)</t>
   </si>
@@ -160,6 +160,15 @@
   </si>
   <si>
     <t>Fahrräder</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>MQ 6.1</t>
+  </si>
+  <si>
+    <t>MQ 5.1</t>
   </si>
 </sst>
 </file>
@@ -477,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,6 +714,22 @@
         <v>42</v>
       </c>
     </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>